<commit_message>
Fix: Database connection and environment variables
- Added dotenv loading to helpers.py and radius_parser.py
- Created systemd-compatible .env.systemd file
- Fixed all DB_CONFIG to use os.environ.get()
- Role-based navigation (viewers only see Lookup)
- Added flash import for password reset
</commit_message>
<xml_diff>
--- a/data/nmp_master.xlsx
+++ b/data/nmp_master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F446"/>
+  <dimension ref="A1:F450"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12914,10 +12914,8 @@
       <c r="F445" t="inlineStr"/>
     </row>
     <row r="446">
-      <c r="A446" t="inlineStr">
-        <is>
-          <t>7165251</t>
-        </is>
+      <c r="A446" t="n">
+        <v>7165251</v>
       </c>
       <c r="B446" t="inlineStr">
         <is>
@@ -12940,6 +12938,112 @@
         </is>
       </c>
       <c r="F446" t="inlineStr"/>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>6834167</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>DIGG</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>2025-05-02 16:00:18</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>live_api</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr"/>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>6834167</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>DIGG</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>2025-05-02 16:00:18</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>live_api</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr"/>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>6406900</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>GTTG</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>2025-03-31 14:37:11</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>live_api</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr"/>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>6406900</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>GTTG</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>2025-03-31 14:37:11</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>live_api</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Session complete: All features working
- MSISDN lookup with location & EPT enrichment
- IMEI search (27K+ devices indexed)
- NMP porting data showing correctly
- Role-based navigation
- Database env variables fixed
- Audit logging active
</commit_message>
<xml_diff>
--- a/data/nmp_master.xlsx
+++ b/data/nmp_master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F450"/>
+  <dimension ref="A1:F451"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13018,10 +13018,8 @@
       <c r="F449" t="inlineStr"/>
     </row>
     <row r="450">
-      <c r="A450" t="inlineStr">
-        <is>
-          <t>6406900</t>
-        </is>
+      <c r="A450" t="n">
+        <v>6406900</v>
       </c>
       <c r="B450" t="inlineStr">
         <is>
@@ -13044,6 +13042,34 @@
         </is>
       </c>
       <c r="F450" t="inlineStr"/>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>7187556</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>ENTG</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>2023-10-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>live_api</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>